<commit_message>
Release 0.3.2 (Set 28, 2024) =================================
* Add revision history
</commit_message>
<xml_diff>
--- a/doc/upm_result_demo.xlsx
+++ b/doc/upm_result_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anniechen/PycharmProjects/myblog/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC78CF5-2779-2845-814B-60E1DBC474C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B33ECD-5450-8C47-BFF9-9B2CFE5A3245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="15800" activeTab="1" xr2:uid="{8A0035D0-D7F0-9240-960B-31838359B463}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>Vendor</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -234,19 +234,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -262,19 +279,25 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -303,23 +326,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>93325</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>175065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2">
+        <xdr:cNvPr id="4" name="图片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7864029-AAE9-916E-B485-409853CD0BED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E814E572-67A6-EC39-4B51-8828DCCBCFAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -335,8 +358,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="203200"/>
-          <a:ext cx="7772400" cy="4766925"/>
+          <a:off x="1651000" y="609600"/>
+          <a:ext cx="7772400" cy="6880665"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -665,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BB935-D0DB-784C-8640-56F75B599E3C}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <selection sqref="A1:G18"/>
+    <sheetView topLeftCell="A16" zoomScale="110" workbookViewId="0">
+      <selection activeCell="G26" sqref="A1:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -683,359 +706,479 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="24">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="2" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="24">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7">
-        <v>4000</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="10">
+        <v>4400</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>56</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="3" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7">
-        <v>4400</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10">
+        <v>4800</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>3820</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>8</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="3" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="7">
+        <v>5200</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24">
+      <c r="A12" s="10"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24">
+      <c r="A13" s="10"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24">
+      <c r="A15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4400</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="24">
+      <c r="A16" s="12"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="24">
+      <c r="A17" s="12"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="24">
+      <c r="A18" s="12"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="24">
+      <c r="A19" s="12"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7">
         <v>4800</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5">
+        <v>308</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="24">
+      <c r="A20" s="12"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="24">
+      <c r="A21" s="12"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="24">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="3" t="s">
+      <c r="F21" s="3">
+        <v>22</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="24">
+      <c r="A22" s="12"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="24">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="7">
-        <v>4000</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="24">
+      <c r="A23" s="12"/>
+      <c r="B23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="7">
+        <v>5200</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="24">
+      <c r="A24" s="12"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="24">
+      <c r="A25" s="12"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="24">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="3" t="s">
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="24">
+      <c r="A26" s="12"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="24">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9">
-        <v>4400</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="6">
-        <v>308</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="24">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="24">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="4">
-        <v>22</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="24">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="24">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" ht="24">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A3:A14"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B13:B18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1047,7 +1190,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>